<commit_message>
feat(data): mark Tmin variable as not to be tuned and add proper colnames
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables_plants20_2y.xlsx
+++ b/JupyterNotebooks/variables_plants20_2y.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BEF594-B85F-4AC8-AAEE-9FAC1C678A01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48416955-8C2A-4673-9A79-5E7B4053057B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -100,19 +100,22 @@
     <t>Cyclotella Nana</t>
   </si>
   <si>
-    <t>Hard Low Border</t>
-  </si>
-  <si>
-    <t>Soft Low Border</t>
-  </si>
-  <si>
-    <t>Soft High Border</t>
-  </si>
-  <si>
-    <t>Hard High Border</t>
-  </si>
-  <si>
     <t>"TMin"</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Hard Min</t>
+  </si>
+  <si>
+    <t>Soft Min</t>
+  </si>
+  <si>
+    <t>Soft Max</t>
+  </si>
+  <si>
+    <t>Hard Max</t>
   </si>
 </sst>
 </file>
@@ -464,19 +467,19 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.83984375" customWidth="1"/>
+    <col min="4" max="4" width="19.578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,20 +501,20 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -538,7 +541,7 @@
       </c>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -563,7 +566,7 @@
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -588,7 +591,7 @@
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -613,7 +616,7 @@
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -640,7 +643,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -663,7 +666,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -686,7 +689,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -713,7 +716,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -740,7 +743,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -763,7 +766,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -788,7 +791,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -813,7 +816,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -821,10 +824,10 @@
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -838,7 +841,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -865,7 +868,7 @@
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -894,7 +897,7 @@
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -923,7 +926,7 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -952,7 +955,7 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -979,7 +982,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1011,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1035,10 +1038,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(data): update hard boarders for 2 year variables
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables_plants20_2y.xlsx
+++ b/JupyterNotebooks/variables_plants20_2y.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48416955-8C2A-4673-9A79-5E7B4053057B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12698EC-3FB1-49AC-8818-DAF0CB7CB311}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
@@ -467,19 +467,19 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="3" width="25.83984375" customWidth="1"/>
-    <col min="4" max="4" width="19.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="19.26171875" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -541,7 +541,7 @@
       </c>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -566,7 +566,7 @@
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -591,7 +591,7 @@
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -614,9 +614,11 @@
       <c r="J5" s="8">
         <v>0.76</v>
       </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -643,7 +645,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -666,7 +668,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -687,9 +689,11 @@
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -716,7 +720,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -743,7 +747,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -766,7 +770,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -791,7 +795,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -816,7 +820,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -841,7 +845,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -868,7 +872,7 @@
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -897,7 +901,7 @@
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -926,7 +930,7 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -955,7 +959,7 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -982,7 +986,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +1015,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1038,10 +1042,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
   </sheetData>

</xml_diff>